<commit_message>
add class and header files
</commit_message>
<xml_diff>
--- a/클래스 세부사항.xlsx
+++ b/클래스 세부사항.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Terratrias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEB6D70-7D85-4255-8D8E-EA5CE4595DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BC0575-A96D-4734-A81B-1E461C55A184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D10E270B-6F85-4ABF-8FC8-9C5E5C84595C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Manager</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,6 +161,10 @@
   </si>
   <si>
     <t>void move(int direction)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int direction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -527,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EE1345-90B8-4B01-90C3-11FC21C869C8}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -648,6 +652,9 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
       <c r="D19" t="s">
         <v>30</v>
       </c>

</xml_diff>